<commit_message>
Improving demos for fitting tension-pCa
</commit_message>
<xml_diff>
--- a/code/demos/fitting/single_tension_pCa/target_data/target_force_pCa_data.xlsx
+++ b/code/demos/fitting/single_tension_pCa/target_data/target_force_pCa_data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ken\GitHub\CampbellMuscleLab\models\MATMyoSim\code\demos\fitting\simple_tension_pCa\target_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ken\Github\CampbellMuscleLab\Models\MATMyoSim\code\demos\fitting\single_tension_pCa\target_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B161FB-0105-44DA-941C-7A1F3E9B53AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1650" windowWidth="24915" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="1650" windowWidth="24915" windowHeight="13950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>SL</t>
   </si>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -393,19 +392,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" customWidth="1"/>
-    <col min="4" max="5" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.265625" customWidth="1"/>
+    <col min="2" max="2" width="3.73046875" customWidth="1"/>
+    <col min="3" max="3" width="4.3984375" customWidth="1"/>
+    <col min="4" max="5" width="11.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -450,13 +449,13 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="D3">
-        <v>623.33333333333337</v>
+        <v>1420</v>
       </c>
       <c r="E3">
-        <v>254.58026457506702</v>
+        <v>738.66997592519851</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -467,13 +466,13 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="D4">
-        <v>890</v>
+        <v>3833.3333333333335</v>
       </c>
       <c r="E4">
-        <v>389.74350539810155</v>
+        <v>1518.1823927900687</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -484,13 +483,13 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>5.6</v>
+        <v>5.2</v>
       </c>
       <c r="D5">
-        <v>1420</v>
+        <v>15243.333333333334</v>
       </c>
       <c r="E5">
-        <v>738.66997592519851</v>
+        <v>1556.5917183956037</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -501,65 +500,23 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="D6">
-        <v>3833.3333333333335</v>
+        <v>24403.333333333332</v>
       </c>
       <c r="E6">
-        <v>1518.1823927900687</v>
+        <v>2227.0633379208398</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>5.2</v>
-      </c>
-      <c r="D7">
-        <v>15243.333333333334</v>
-      </c>
-      <c r="E7">
-        <v>1556.5917183956037</v>
-      </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>23963.333333333332</v>
-      </c>
-      <c r="E8">
-        <v>2777.056795322063</v>
-      </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>4.8</v>
-      </c>
-      <c r="D9">
-        <v>24403.333333333332</v>
-      </c>
-      <c r="E9">
-        <v>2227.0633379208398</v>
-      </c>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" s="1"/>
@@ -642,17 +599,8 @@
     <row r="36" spans="2:2">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="1"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E39">
+  <sortState ref="A2:E39">
     <sortCondition descending="1" ref="C2:C39"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>